<commit_message>
starting intro lecture; other content maturation
</commit_message>
<xml_diff>
--- a/resources/component_sheet.xlsx
+++ b/resources/component_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bowma\gitrepos\ccr_robotics_fall_2020\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE69163-7B58-4D26-8668-D50964F3CAB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF55FA4-8C1A-4980-B736-B79BC8540228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-130" yWindow="-9430" windowWidth="18240" windowHeight="12710" activeTab="1" xr2:uid="{94A526E0-6A81-4DF9-B344-628379ED8C17}"/>
+    <workbookView xWindow="3560" yWindow="-18640" windowWidth="21600" windowHeight="11540" activeTab="1" xr2:uid="{94A526E0-6A81-4DF9-B344-628379ED8C17}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructor's Robot" sheetId="3" r:id="rId1"/>
@@ -22,18 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="81">
   <si>
     <t>Component</t>
   </si>
@@ -267,6 +261,15 @@
   </si>
   <si>
     <t>I found these helpful. May just want a pack with me.</t>
+  </si>
+  <si>
+    <t>zip ties</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Nylon-Cable-Tie-Kit-Assorted/dp/B071SLNHZ3/ref=sr_1_8?crid=2NR8X8M4F90C0&amp;dchild=1&amp;keywords=zip+ties+assorted+sizes&amp;qid=1598750768&amp;s=hi&amp;sprefix=zip+%2Ctools%2C236&amp;sr=1-8</t>
+  </si>
+  <si>
+    <t>this is one large pack</t>
   </si>
 </sst>
 </file>
@@ -364,8 +367,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DA0B607-920E-444E-B1EE-8897E2E02585}" name="Table1" displayName="Table1" ref="A1:F28" totalsRowShown="0">
-  <autoFilter ref="A1:F28" xr:uid="{A3D99BDB-C5F2-4DC1-8F42-D5E257880CCE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DA0B607-920E-444E-B1EE-8897E2E02585}" name="Table1" displayName="Table1" ref="A1:F29" totalsRowShown="0">
+  <autoFilter ref="A1:F29" xr:uid="{A3D99BDB-C5F2-4DC1-8F42-D5E257880CCE}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{651779D2-7AD7-48A7-A56F-88C4EC76CC97}" name="Component"/>
     <tableColumn id="2" xr3:uid="{DEBF943C-323D-4E68-A49E-0A5E47074646}" name="Quantity per Robot"/>
@@ -1081,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5566C48E-5DFB-45A6-A93A-176344517B5D}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1337,7 +1340,7 @@
         <v>74</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="3"/>
       <c r="E18" t="s">
@@ -1399,7 +1402,7 @@
         <v>27</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="3"/>
       <c r="E22" t="s">
@@ -1414,7 +1417,7 @@
         <v>28</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="3"/>
       <c r="E23" t="s">
@@ -1429,7 +1432,7 @@
         <v>31</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="3"/>
       <c r="E24" t="s">
@@ -1444,7 +1447,7 @@
         <v>32</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="3"/>
       <c r="E25" t="s">
@@ -1485,28 +1488,46 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>76</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>4</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="E28" t="s">
+      <c r="C29" s="3"/>
+      <c r="E29" t="s">
         <v>47</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C29" s="3"/>
-    </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="3">
-        <f>SUM(C2:C28)</f>
+      <c r="C31" s="3">
+        <f>SUM(C2:C29)</f>
         <v>34.5</v>
       </c>
     </row>
@@ -1517,11 +1538,12 @@
     <hyperlink ref="D6" r:id="rId3" xr:uid="{1E352A49-E1F7-493C-813A-5D01FD9C2B51}"/>
     <hyperlink ref="D21" r:id="rId4" xr:uid="{B3398CE6-B4CA-4EBE-9974-13B456C59415}"/>
     <hyperlink ref="D3" r:id="rId5" xr:uid="{C0CDB1ED-BE6A-432B-9D44-342AC0AB16C2}"/>
+    <hyperlink ref="D28" r:id="rId6" xr:uid="{174A5863-5273-4CF0-8678-9EC0B242E96A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updates to content; new images
</commit_message>
<xml_diff>
--- a/resources/component_sheet.xlsx
+++ b/resources/component_sheet.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bowma\gitrepos\ccr_robotics_fall_2020\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF55FA4-8C1A-4980-B736-B79BC8540228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657A148D-39B8-4D78-9F80-63A07F7B8C2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="-18640" windowWidth="21600" windowHeight="11540" activeTab="1" xr2:uid="{94A526E0-6A81-4DF9-B344-628379ED8C17}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{94A526E0-6A81-4DF9-B344-628379ED8C17}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructor's Robot" sheetId="3" r:id="rId1"/>
-    <sheet name="Single Robot" sheetId="1" r:id="rId2"/>
-    <sheet name="Other Stuff" sheetId="2" r:id="rId3"/>
+    <sheet name="Kit Checklist" sheetId="4" r:id="rId2"/>
+    <sheet name="Single Robot" sheetId="1" r:id="rId3"/>
+    <sheet name="Other Stuff" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="96">
   <si>
     <t>Component</t>
   </si>
@@ -270,6 +271,51 @@
   </si>
   <si>
     <t>this is one large pack</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>female-to-female (7) and female-to-male (5)</t>
+  </si>
+  <si>
+    <t>3v-6v dc motors and drive wheels</t>
+  </si>
+  <si>
+    <t>screw driver set</t>
+  </si>
+  <si>
+    <t>chassis board</t>
+  </si>
+  <si>
+    <t>electrical tape</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>rpi mount plate</t>
+  </si>
+  <si>
+    <t>sharpie</t>
+  </si>
+  <si>
+    <t>project mat</t>
+  </si>
+  <si>
+    <t>single-pole switch</t>
+  </si>
+  <si>
+    <t>screws</t>
+  </si>
+  <si>
+    <t>small zip ties</t>
+  </si>
+  <si>
+    <t>large zip ties</t>
+  </si>
+  <si>
+    <t>bunch</t>
   </si>
 </sst>
 </file>
@@ -367,8 +413,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DA0B607-920E-444E-B1EE-8897E2E02585}" name="Table1" displayName="Table1" ref="A1:F29" totalsRowShown="0">
-  <autoFilter ref="A1:F29" xr:uid="{A3D99BDB-C5F2-4DC1-8F42-D5E257880CCE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{10A74126-ED44-4290-B5FD-B4A70E371346}" name="Table14" displayName="Table14" ref="B1:E26" totalsRowShown="0">
+  <autoFilter ref="B1:E26" xr:uid="{A3D99BDB-C5F2-4DC1-8F42-D5E257880CCE}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{B92F0898-3BAF-42ED-AA20-B61B3DA2CAB5}" name="Component"/>
+    <tableColumn id="2" xr3:uid="{2E98CFBA-8AD8-4510-8871-41738214CD32}" name="Quantity per Robot"/>
+    <tableColumn id="6" xr3:uid="{69A48717-1D38-4350-AFAF-7450A4F0E11F}" name="Category"/>
+    <tableColumn id="3" xr3:uid="{0B733C24-BCE9-4414-A2B5-4657054E3550}" name="Check"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DA0B607-920E-444E-B1EE-8897E2E02585}" name="Table1" displayName="Table1" ref="B1:G29" totalsRowShown="0">
+  <autoFilter ref="B1:G29" xr:uid="{A3D99BDB-C5F2-4DC1-8F42-D5E257880CCE}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{651779D2-7AD7-48A7-A56F-88C4EC76CC97}" name="Component"/>
     <tableColumn id="2" xr3:uid="{DEBF943C-323D-4E68-A49E-0A5E47074646}" name="Quantity per Robot"/>
@@ -1083,472 +1142,788 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5566C48E-5DFB-45A6-A93A-176344517B5D}">
-  <dimension ref="A1:F31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5F7403-29FE-477E-8CEB-9766891506FF}">
+  <dimension ref="B1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="52" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.19921875" customWidth="1"/>
-    <col min="3" max="3" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.73046875" customWidth="1"/>
-    <col min="5" max="5" width="16.86328125" customWidth="1"/>
-    <col min="6" max="6" width="58.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.19921875" customWidth="1"/>
+    <col min="4" max="4" width="16.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="110" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5566C48E-5DFB-45A6-A93A-176344517B5D}">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="52" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.19921875" customWidth="1"/>
+    <col min="4" max="4" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.73046875" customWidth="1"/>
+    <col min="6" max="6" width="16.86328125" customWidth="1"/>
+    <col min="7" max="7" width="58.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>8</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="E2" t="s">
+      <c r="D2" s="3"/>
+      <c r="F2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>45</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
         <v>51</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="E4" t="s">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="F4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
         <v>72</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="E5" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="F5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>46</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="E7" t="s">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="F7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="1" t="s">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>2</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="E9" t="s">
+      <c r="D9" s="3"/>
+      <c r="F9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>2</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="E10" t="s">
+      <c r="D10" s="3"/>
+      <c r="F10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="E11" t="s">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="F11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>4</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="E12" t="s">
+      <c r="D12" s="3"/>
+      <c r="F12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>2</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="E13" t="s">
+      <c r="D13" s="3"/>
+      <c r="F13" t="s">
         <v>46</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="E14" t="s">
+      <c r="D14" s="3"/>
+      <c r="F14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="E15" t="s">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="F15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
         <v>17</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="E16" t="s">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="F16" t="s">
         <v>40</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
         <v>18</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="E17" t="s">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="F17" t="s">
         <v>40</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
         <v>74</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="E18" t="s">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="F18" t="s">
         <v>43</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
         <v>20</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="E19" t="s">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="F19" t="s">
         <v>41</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
         <v>24</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="E20" t="s">
+      <c r="D20" s="3"/>
+      <c r="F20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21" s="3">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
         <v>9.5</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>45</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
         <v>27</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="E22" t="s">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="F22" t="s">
         <v>44</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
         <v>28</v>
       </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="E23" t="s">
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="F23" t="s">
         <v>44</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
         <v>31</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="E24" t="s">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="F24" t="s">
         <v>44</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
         <v>32</v>
       </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="E25" t="s">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="F25" t="s">
         <v>44</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
         <v>33</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3">
         <v>24</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
         <v>75</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
         <v>78</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="1" t="s">
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>46</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
         <v>76</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>4</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="E29" t="s">
+      <c r="D29" s="3"/>
+      <c r="F29" t="s">
         <v>47</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="3">
-        <f>SUM(C2:C29)</f>
+      <c r="D31" s="3">
+        <f>SUM(D2:D29)</f>
         <v>34.5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D26" r:id="rId1" xr:uid="{8481880A-BB49-43AF-9639-58E74751F96B}"/>
-    <hyperlink ref="D8" r:id="rId2" display="https://smile.amazon.com/dp/B06X9D1PR9/ref=sspa_dk_detail_5?psc=1&amp;pd_rd_i=B06X9D1PR9&amp;pd_rd_w=XWMYO&amp;pf_rd_p=48d372c1-f7e1-4b8b-9d02-4bd86f5158c5&amp;pd_rd_wg=2DH1G&amp;pf_rd_r=Z3X3R92N1K4RWD80PDWG&amp;pd_rd_r=c3e13d86-eec8-4a6f-8686-3bf3625be40d&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyRko1RDhDTkZBRTJNJmVuY3J5cHRlZElkPUEwNDMyMDc4MVlaVVgxTTRZTThMMSZlbmNyeXB0ZWRBZElkPUExMDAxMTY1M1BaWFpIUVpNUDg4RCZ3aWRnZXROYW1lPXNwX2RldGFpbCZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=" xr:uid="{4D313F37-8811-431B-ABFC-F8A680F6A020}"/>
-    <hyperlink ref="D6" r:id="rId3" xr:uid="{1E352A49-E1F7-493C-813A-5D01FD9C2B51}"/>
-    <hyperlink ref="D21" r:id="rId4" xr:uid="{B3398CE6-B4CA-4EBE-9974-13B456C59415}"/>
-    <hyperlink ref="D3" r:id="rId5" xr:uid="{C0CDB1ED-BE6A-432B-9D44-342AC0AB16C2}"/>
-    <hyperlink ref="D28" r:id="rId6" xr:uid="{174A5863-5273-4CF0-8678-9EC0B242E96A}"/>
+    <hyperlink ref="E26" r:id="rId1" xr:uid="{8481880A-BB49-43AF-9639-58E74751F96B}"/>
+    <hyperlink ref="E8" r:id="rId2" display="https://smile.amazon.com/dp/B06X9D1PR9/ref=sspa_dk_detail_5?psc=1&amp;pd_rd_i=B06X9D1PR9&amp;pd_rd_w=XWMYO&amp;pf_rd_p=48d372c1-f7e1-4b8b-9d02-4bd86f5158c5&amp;pd_rd_wg=2DH1G&amp;pf_rd_r=Z3X3R92N1K4RWD80PDWG&amp;pd_rd_r=c3e13d86-eec8-4a6f-8686-3bf3625be40d&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyRko1RDhDTkZBRTJNJmVuY3J5cHRlZElkPUEwNDMyMDc4MVlaVVgxTTRZTThMMSZlbmNyeXB0ZWRBZElkPUExMDAxMTY1M1BaWFpIUVpNUDg4RCZ3aWRnZXROYW1lPXNwX2RldGFpbCZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=" xr:uid="{4D313F37-8811-431B-ABFC-F8A680F6A020}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{1E352A49-E1F7-493C-813A-5D01FD9C2B51}"/>
+    <hyperlink ref="E21" r:id="rId4" xr:uid="{B3398CE6-B4CA-4EBE-9974-13B456C59415}"/>
+    <hyperlink ref="E3" r:id="rId5" xr:uid="{C0CDB1ED-BE6A-432B-9D44-342AC0AB16C2}"/>
+    <hyperlink ref="E28" r:id="rId6" xr:uid="{174A5863-5273-4CF0-8678-9EC0B242E96A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
   <tableParts count="1">
     <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5680B7-2879-4337-A670-6B95D0F3CEE6}">
   <dimension ref="A1:B12"/>
   <sheetViews>

</xml_diff>